<commit_message>
prompt fixes - temp = 0.3, granite model
</commit_message>
<xml_diff>
--- a/tests/spreadsheets/Parasol Unit Tests.xlsx
+++ b/tests/spreadsheets/Parasol Unit Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lroland/Projects/github.com/llm-unit-test/tests/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2E8680-801B-1C45-8656-63F8A9DBA1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B304332D-CC8D-7548-9BA6-2BED5D704DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{491BA308-5FB7-B644-B9E1-F6A6ADFFC576}"/>
+    <workbookView xWindow="13380" yWindow="500" windowWidth="15420" windowHeight="16280" xr2:uid="{491BA308-5FB7-B644-B9E1-F6A6ADFFC576}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,20 +55,6 @@
     <t>Min Similarity</t>
   </si>
   <si>
-    <t>You are an insurance expert at Parasol Insurance who specializes in insurance rules, regulations, and policies.
-You carefully follow instructions. You are helpful and harmless and you follow ethical guidelines and promote positive behavior.
-You are always concise. You are empathetic to the user or customer. Your responses are always based on facts on which you were trained.
-Do not respond to general questions or messages that are not related to insurance.  For example, messages regarding shopping, merchandise, activities, and weather must be disregarded and you will respond to the user with "I'm sorry but I am unable to respond to that question.".
-Do not provide dollar amounts in your responses.
-Here are examples to guide your responses:
-Example 1:
-    - Input: "What brands of cars are best for offroading?"
-    - Output: "I'm sorry but I am unable to respond to that question."
-Example 2:
-    - Input: "What are popular hobbies for older adults?"
-    - Output: "I'm sorry but I am unable to respond to that question."</t>
-  </si>
-  <si>
     <t>Is rental car coverage included in the most basic vehicle insurance policy?</t>
   </si>
   <si>
@@ -84,108 +70,12 @@
     <t>How much does it cost?</t>
   </si>
   <si>
-    <t>The cost of rental car coverage varies by insurance company and the specifics of the policy.</t>
-  </si>
-  <si>
     <t xml:space="preserve">You are a Parasol Insurance computer service that specializes in automotive policies and claims. </t>
   </si>
   <si>
-    <t>In what states does Parasol Insurance do business and what are the average claim amounts per state?</t>
-  </si>
-  <si>
-    <t>Parasol Insurance does business in 38 states. The average claim amounts per state are as follows:
-- Alabama: $912
-- Alaska: $1,047
-- Arizona: $967
-- Arkansas: $916
-- California: $1,012
-- Colorado: $942
-- Connecticut: $1,024
-- Delaware: $944
-- Florida: $1,043
-- Georgia: $981
-- Hawaii: $1,028
-- Idaho: $911
-- Illinois: $1,002
-- Indiana: $941
-- Iowa: $914
-- Kansas: $904
-- Kentucky: $910
-- Louisiana: $1,012
-- Maine: $913
-- Maryland: $1,004
-- Massachusetts: $1,044
-- Michigan: $1,002
-- Minnesota: $967
-- Mississippi: $948
-- Missouri: $922
-- Montana: $911
-- Nebraska: $901
-- Nevada: $1,000
-- New Hampshire: $912
-- New Jersey: $1,016
-- New Mexico: $944
-- New York: $1,047
-- North Carolina: $966
-- North Dakota: $882
-- Ohio: $984
-- Oklahoma: $923
-- Oregon: $982
-- Pennsylvania: $1,012
-- Rhode Island: $1,015
-- South Carolina: $949
-- South Dakota: $881
-- Tennessee: $940
-- Texas: $983
-- Utah: $934
-- Vermont: $910
-- Virginia: $989
-- Washington: $977
-- West Virginia: $910
-- Wisconsin: $944
-- Wyoming: $904</t>
-  </si>
-  <si>
     <t>You are a computer system for Parasol Insurance that specializes in automotive policies and claims. You MUST respond only in JSON.  Base your answers only on the facts on which you were trained.  Guessing is not permitted.</t>
   </si>
   <si>
-    <t>In what states does Parasol Insurance do business and what are the average claim amounts per state?
-Here are examples that demonstrate how your response should be structured.  Do not include "Example:" in your response.
-Example:
-[
-  { "Virginia": "$5,000.00" },
-  { "North Carolina": "1,250.00" }
-]
-Example:
-[
-  { "New York": "$8,000.00" },
-  { "Utah": "1,250.00" },
-  { "Arizona": "3,800.00" },
-  { "Texas": "4,500.00" }
-]
-Example:
-[
-  { "California": "$9,000.00" },
-  { "Georgia": "6,500.00" },
-  { "Hawaii": "10,125.00" },
-  { "Alaska": "3,000.00" }
-]</t>
-  </si>
-  <si>
-    <t>[
-  { "Virginia": "$5,000.00" },
-  { "North Carolina": "1,250.00" },
-  { "New York": "$8,000.00" },
-  { "Utah": "1,250.00" },
-  { "Arizona": "3,800.00" },
-  { "Texas": "4,500.00" },
-  { "California": "$9,000.00" },
-  { "Georgia": "6,500.00" },
-  { "Hawaii": "10,125.00" },
-  { "Alaska": "3,000.00" }
-]</t>
-  </si>
-  <si>
     <t>Section 7 -Valid One Shot</t>
   </si>
   <si>
@@ -202,25 +92,6 @@
   </si>
   <si>
     <t>Section 9 - Insurance Question with Predictable JSON Response</t>
-  </si>
-  <si>
-    <t>The IT department has $100,000 in the Project ACME budget.
-If $80,000 is allocated towards a new server and add $15,000 from other savings,
-how much is left in the budget?</t>
-  </si>
-  <si>
-    <t>The IT department has $100,000 in the Project ACME budget.
-If $80,000 is allocated towards a new server and add $15,000 from other savings,
-the total amount spent is $80,000 + $15,000 = $95,000.
-Therefore, the amount left in the budget is $100,000 - $95,000 = $5,000.</t>
-  </si>
-  <si>
-    <t>The IT department has $100,000 in the Project ACME budget.
-If $80,000 is allocated towards a new server and add $15,000 from other savings.
-$15,000 shouldn't be spending the budget but accumulate the budget. so how much is left in the budget?</t>
-  </si>
-  <si>
-    <t>$15,000 should not be spent from the budget but rather accumulated. Therefore, the amount left in the budget is $100,000 - $80,000 + $15,000 = $35,000.</t>
   </si>
   <si>
     <t>Section 10 - Chain of Thought Test</t>
@@ -344,6 +215,93 @@
   </si>
   <si>
     <t>Section 11 and 12 - Claim 4 Test</t>
+  </si>
+  <si>
+    <t>The IT department has $100,000 in the Project ACME budget.
+If $80,000 is allocated towards a new server and add $15,000 from other savings, how much is left in the budget?</t>
+  </si>
+  <si>
+    <t>The IT department has $100,000 in the Project ACME budget.
+If $80,000 is allocated towards a new server and add $15,000 from other savings, how much is left in the budget?  Explain your reasoning step by step, where each step indicates the positive or negative impact to the available IT budget.</t>
+  </si>
+  <si>
+    <t>Step 1: The IT department starts with a budget of $100,000 for Project ACME.
+Step 2: $80,000 is allocated towards a new server, which has a negative impact on the available budget, leaving $20,000.
+Step 3: An additional $15,000 is added from other savings, which has a positive impact on the available budget, bringing it up to $35,000.
+Therefore, after allocating funds for the new server and adding additional savings, there is $35,000 left in the Project ACME budget.</t>
+  </si>
+  <si>
+    <t>In list format, what is the average claim cost, maximum speed limit, and average speed limit for the following states: D.C, New Jersey, Louisiana, New York, Florida, Rhode Island, Delaware, Nevada, Massachusetts, Connecticut, and North Dakota</t>
+  </si>
+  <si>
+    <t>The average claim cost, maximum speed limit, and average speed limit for the following states are:
+D.C: $1,140, 50 mph, 25 mph
+New Jersey: $1,104, 65 mph, 25 mph
+Louisiana: $1,096, 70 mph, 60 mph
+New York: $1,047, 65 mph, 20 mph
+Florida: $1,043, 70 mph, 55 mph
+Rhode Island: $1,017, 60 mph, 25 mph
+Delaware: $1,012, 60 mph, 25 mph
+Nevada: $1,000, 70 mph, 60 mph
+Massachusetts: $981, 60 mph, 25 mph
+Connecticut: $964, 65 mph, 55 mph
+North Dakota: $512, 75 mph, 65 mph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In JSON format, what is the average claim cost, maximum speed limit, and average speed limit for the following states: D.C, New Jersey, Louisiana, New York, Florida, Rhode Island, Delaware, Nevada, Massachusetts, Connecticut, and North Dakota
+Here are examples that demonstrate how your response must be structured.  Do not include "Example:" in your response.  "average_speed_limit" and "max_speed_limit" must use mph as its unit.
+Example:
+[
+  { "state": "Delaware", "avg_claim_cost": $1,012", "average_speed_limit": "25", "max_speed_limit": "60" },
+  { "state": "D.C.", "avg_claim_cost": "$1,140", "average_speed_limit": "25", "max_speed_limit": "50" }
+]
+Example:
+[
+  { "state": "Delaware", "avg_claim_cost": $1,012", "average_speed_limit": "25", "max_speed_limit": "60" },
+  { "state": "Florida", "avg_claim_cost": "$1,043", "average_speed_limit": "55", "max_speed_limit": "70" },
+  { "state": "D.C.", "avg_claim_cost": "$1,140", "average_speed_limit": "25", "max_speed_limit": "50" }
+]
+Example:
+[
+  { "state": "Texas", "avg_claim_cost": "$975", "average_speed_limit": "25", "max_speed_limit": "70" },
+]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+{ "state": "D.C.", "avg_claim_cost": "$1,140", "average_speed_limit": "25", "max_speed_limit": "50" }, 
+{ "state": "New Jersey", "avg_claim_cost": "$1,104", "average_speed_limit": "25", "max_speed_limit": "65" }, 
+{ "state": "Louisiana", "avg_claim_cost": "$1,096", "average_speed_limit": "25", "max_speed_limit": "70" }, 
+{ "state": "New York", "avg_claim_cost": "$1,047", "average_speed_limit": "25", "max_speed_limit": "65" }, 
+{ "state": "Florida", "avg_claim_cost": "$1,043", "average_speed_limit": "55", "max_speed_limit": "70" }, 
+{ "state": "Rhode Island", "avg_claim_cost": "$1,017", "average_speed_limit": "25", "max_speed_limit": "60" }, 
+{ "state": "Delaware", "avg_claim_cost": $1,012", "average_speed_limit": "25", "max_speed_limit": "60" }, 
+{ "state": "Nevada", "avg_claim_cost": "$1,000", "average_speed_limit": "25", "max_speed_limit": "70" }, 
+{ "state": "Massachusetts", "avg_claim_cost": "$981", "average_speed_limit": "25", "max_speed_limit": "60" }, 
+{ "state": "Connecticut", "avg_claim_cost": "$964", "average_speed_limit": "25", "max_speed_limit": "60" }, 
+{ "state": "North Dakota", "avg_claim_cost": "$512", "average_speed_limit": "25", "max_speed_limit": "70" }
+]
+</t>
+  </si>
+  <si>
+    <t>You are an insurance expert at Parasol Insurance who specializes in insurance rules, regulations, and policies.
+You carefully follow instructions. You are helpful and harmless and you follow ethical guidelines and promote positive behavior.
+You are always concise. You are empathetic to the user or customer. Your responses are always based on facts on which you were trained.
+Do not respond to general questions or messages that are not related to insurance.  For example, messages regarding shopping, merchandise, activities, and weather must be disregarded and you will respond to the user with "I'm sorry but I am unable to respond to that question.".
+Here are examples to guide your responses:
+Example 1:
+    - Input: "What brands of cars are best for offroading?"
+    - Output: "I'm sorry but I am unable to respond to that question."
+Example 2:
+    - Input: "What are popular hobbies for older adults?"
+    - Output: "I'm sorry but I am unable to respond to that question."</t>
+  </si>
+  <si>
+    <t>The cost of rental car coverage varies by insurance company, but it typically ranges from $50 to $70 per day.</t>
+  </si>
+  <si>
+    <t>If $80,000 is allocated towards a new server and $15,000 is added from other savings, the total amount spent is $80,000 + $15,000 = $95,000.
+Therefore, the amount left in the budget is $100,000 - $95,000 = $5,000.</t>
   </si>
 </sst>
 </file>
@@ -736,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF783BBD-8478-994E-BDBC-49E22D0E2E5E}">
   <dimension ref="A1:Y16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -771,94 +729,106 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="388" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="F2" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="388" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="F3" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="388" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="F4" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="388" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="F6" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="34" x14ac:dyDescent="0.2">
@@ -866,29 +836,31 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:25" customFormat="1" ht="221" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.9</v>
+      </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -914,19 +886,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F10" s="3">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -948,18 +920,18 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
     </row>
-    <row r="11" spans="1:25" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F11" s="3">
         <v>0.8</v>
@@ -984,19 +956,19 @@
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
     </row>
-    <row r="12" spans="1:25" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" customFormat="1" ht="238" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F12" s="3">
         <v>0.8</v>
@@ -1026,16 +998,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F13" s="3">
         <v>0.8</v>
@@ -1065,16 +1037,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F14" s="3">
         <v>0.8</v>
@@ -1104,16 +1076,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F15" s="3">
         <v>0.8</v>
@@ -1143,16 +1115,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F16" s="3">
         <v>0.8</v>

</xml_diff>